<commit_message>
Updated parent config code for results, filters, conditions
Added functionality for resultgrades, saved filters, and detection conditions
</commit_message>
<xml_diff>
--- a/utils/config/ReferenceLists/projects.xlsx
+++ b/utils/config/ReferenceLists/projects.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/jeremy_krogh_gov_bc_ca/Documents/Projects/2023/EMStoSamples/CanadaTestConfiguration/Projects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/sahil_bhandari_gov_bc_ca/Documents/teamdocs/GitHub/aqs-api/utils/config/ReferenceLists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="11_F25DC773A252ABDACC104892899E443A5ADE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6777E14-BF99-4E49-915B-49A4FB5636AD}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="11_F25DC773A252ABDACC104892899E443A5ADE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E43E6A28-43BC-4094-9424-AF3FCD33C265}"/>
   <bookViews>
-    <workbookView xWindow="-14025" yWindow="-16440" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="projects" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -471,15 +471,15 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="59.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="102.7109375" customWidth="1"/>
-    <col min="7" max="7" width="115.28515625" customWidth="1"/>
+    <col min="2" max="2" width="59.453125" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="102.7265625" customWidth="1"/>
+    <col min="7" max="7" width="115.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -502,7 +502,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -522,7 +522,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -542,7 +542,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -563,7 +563,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -574,7 +574,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -588,7 +588,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -602,7 +602,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -616,7 +616,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>

</xml_diff>